<commit_message>
updated gitignore and commited other files
</commit_message>
<xml_diff>
--- a/results_ca2.xlsx
+++ b/results_ca2.xlsx
@@ -3087,13 +3087,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3503,8 +3503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U52" sqref="U52"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>